<commit_message>
Updated Timesheet till 9/2/2012
</commit_message>
<xml_diff>
--- a/TimeSheet.xlsx
+++ b/TimeSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Jan" sheetId="1" r:id="rId1"/>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="32">
   <si>
     <t>Date</t>
   </si>
@@ -659,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -668,7 +668,7 @@
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="50.28515625" customWidth="1"/>
+    <col min="10" max="10" width="62.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10">
@@ -1028,10 +1028,10 @@
         <v>41299</v>
       </c>
       <c r="C31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D31" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:10">
@@ -1039,10 +1039,10 @@
         <v>41300</v>
       </c>
       <c r="C32" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:4">
@@ -1050,10 +1050,10 @@
         <v>41301</v>
       </c>
       <c r="C33" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:4">
@@ -1061,10 +1061,10 @@
         <v>41302</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
-      </c>
-      <c r="D34" t="s">
-        <v>30</v>
+        <v>5</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:4">
@@ -1112,7 +1112,7 @@
   <dimension ref="B3:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1120,7 +1120,7 @@
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="50.28515625" customWidth="1"/>
+    <col min="10" max="10" width="71.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10">
@@ -1149,6 +1149,12 @@
       <c r="B7" s="3">
         <v>41306</v>
       </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
       <c r="I7" s="4" t="s">
         <v>5</v>
       </c>
@@ -1160,6 +1166,12 @@
       <c r="B8" s="3">
         <v>41307</v>
       </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="I8" s="6" t="s">
         <v>7</v>
       </c>
@@ -1171,6 +1183,12 @@
       <c r="B9" s="3">
         <v>41308</v>
       </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
       <c r="I9" s="6" t="s">
         <v>9</v>
       </c>
@@ -1182,6 +1200,12 @@
       <c r="B10" s="3">
         <v>41309</v>
       </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>0.5</v>
+      </c>
       <c r="I10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1193,6 +1217,12 @@
       <c r="B11" s="3">
         <v>41310</v>
       </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
       <c r="I11" s="6" t="s">
         <v>13</v>
       </c>
@@ -1204,6 +1234,12 @@
       <c r="B12" s="3">
         <v>41311</v>
       </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>30</v>
+      </c>
       <c r="I12" s="6" t="s">
         <v>15</v>
       </c>
@@ -1215,6 +1251,12 @@
       <c r="B13" s="3">
         <v>41312</v>
       </c>
+      <c r="C13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
       <c r="I13" s="6" t="s">
         <v>17</v>
       </c>
@@ -1226,6 +1268,12 @@
       <c r="B14" s="3">
         <v>41313</v>
       </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
       <c r="I14" s="6" t="s">
         <v>19</v>
       </c>
@@ -1236,6 +1284,12 @@
     <row r="15" spans="2:10" ht="14.25" customHeight="1">
       <c r="B15" s="3">
         <v>41314</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="I15" s="6" t="s">
         <v>21</v>
@@ -1363,7 +1417,7 @@
   <dimension ref="B3:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1371,7 +1425,7 @@
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="50.28515625" customWidth="1"/>
+    <col min="10" max="10" width="69.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10">
@@ -1628,7 +1682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -1637,7 +1691,7 @@
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" customWidth="1"/>
-    <col min="10" max="10" width="50.28515625" customWidth="1"/>
+    <col min="10" max="10" width="73.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10">

</xml_diff>